<commit_message>
Updated code to read reward plan designs
</commit_message>
<xml_diff>
--- a/clientTestData/JMH.xlsx
+++ b/clientTestData/JMH.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Desktop/prac Clients/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Documents/RallyMochaFramework/clientTestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F616C76-A32E-B849-8C5A-3D6F349D170B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CEB87D-713E-1947-87B4-27A47FF97B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,29 +175,23 @@
     <t>57a8cda4-581c-45b2-8d14-db36b9e71299</t>
   </si>
   <si>
-    <t>John Muir Health - 01/01/2021</t>
-  </si>
-  <si>
     <t>PROD_JMH_AUM_AFF1a@mailinator.com</t>
+  </si>
+  <si>
+    <t>SAIC - 01/01/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -241,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,7 +252,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +569,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -685,7 +678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>25</v>
@@ -699,8 +692,8 @@
       <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>51</v>
+      <c r="F2" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
@@ -729,7 +722,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
updated minor changes to code to optimize the execution
</commit_message>
<xml_diff>
--- a/clientTestData/JMH.xlsx
+++ b/clientTestData/JMH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Desktop/prac Clients/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F616C76-A32E-B849-8C5A-3D6F349D170B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F5858B-D2A1-C549-8716-E7DF5C4B32DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>CUST_ID</t>
   </si>
@@ -109,9 +109,6 @@
     <t>MCCARTHY</t>
   </si>
   <si>
-    <t>CBIZ</t>
-  </si>
-  <si>
     <t>0188335</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>2021.09.01_CBIZ_Aff2_EREPR</t>
   </si>
   <si>
-    <t>uat_HJTfIdXh@rally.mailinator.com</t>
-  </si>
-  <si>
     <t>7fda1573-526a-4be9-a20c-a85b6759be27</t>
   </si>
   <si>
@@ -169,35 +163,26 @@
     <t>LAVENTIS</t>
   </si>
   <si>
-    <t>uat_UuvkNQnr@rally.mailinator.com</t>
-  </si>
-  <si>
     <t>57a8cda4-581c-45b2-8d14-db36b9e71299</t>
   </si>
   <si>
-    <t>John Muir Health - 01/01/2021</t>
-  </si>
-  <si>
     <t>PROD_JMH_AUM_AFF1a@mailinator.com</t>
+  </si>
+  <si>
+    <t>John Muir Health</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -241,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,7 +243,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +560,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -685,7 +669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>25</v>
@@ -699,158 +683,159 @@
       <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>51</v>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="W2" r:id="rId1" display="mailto:PROD_JMH_AUM_AFF1a@mailinator.com" xr:uid="{834C993A-5862-5740-AC6F-A30C9FF78414}"/>
+    <hyperlink ref="W3:W4" r:id="rId2" display="mailto:PROD_JMH_AUM_AFF1a@mailinator.com" xr:uid="{89623699-624B-F647-A03C-1904D4595419}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>